<commit_message>
Added use case diagram and machine state diagram
</commit_message>
<xml_diff>
--- a/docs/Charts.xlsx
+++ b/docs/Charts.xlsx
@@ -8,26 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Formação\05_Mestrado (ISCTE)\1Ano\1Semestre\ADS\PG\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D45804-8D80-4DE5-ACD6-BC473B8FB548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5442231E-9E5B-4B6C-BD97-603A1B378B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{7DEC2CA6-CF89-4290-8B80-2E392530E8C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{7DEC2CA6-CF89-4290-8B80-2E392530E8C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Gestão de riscos" sheetId="2" r:id="rId2"/>
-    <sheet name="Test Check to US" sheetId="3" r:id="rId3"/>
-    <sheet name="BURNDOWN CHART 1ºSprint" sheetId="4" r:id="rId4"/>
-    <sheet name="BURNDOWN CHART 2ºSprint " sheetId="5" r:id="rId5"/>
-    <sheet name="BURNDOWN CHART 3ºSprint " sheetId="6" r:id="rId6"/>
-    <sheet name="BURNDOWN CHART 4ºSprint" sheetId="7" r:id="rId7"/>
-    <sheet name="BURNDOWN CHART 5ºSprint" sheetId="8" r:id="rId8"/>
+    <sheet name="Test Check to US" sheetId="3" r:id="rId1"/>
+    <sheet name="BURNDOWN CHART 1ºSprint" sheetId="4" r:id="rId2"/>
+    <sheet name="BURNDOWN CHART 2ºSprint " sheetId="5" r:id="rId3"/>
+    <sheet name="BURNDOWN CHART 3ºSprint " sheetId="6" r:id="rId4"/>
+    <sheet name="BURNDOWN CHART 4ºSprint" sheetId="7" r:id="rId5"/>
+    <sheet name="BURNDOWN CHART 5ºSprint" sheetId="8" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gestão de riscos'!$B$4:$G$11</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -474,109 +466,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="87">
-  <si>
-    <t>5NOV a 1ODEZ</t>
-  </si>
-  <si>
-    <t>Diagrama de gantt</t>
-  </si>
-  <si>
-    <t>Gestão de Riscos</t>
-  </si>
-  <si>
-    <t>Risco</t>
-  </si>
-  <si>
-    <t>Grau de Impacto</t>
-  </si>
-  <si>
-    <t>Grau de Probabilidade</t>
-  </si>
-  <si>
-    <t>Consequências</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recursos Afetados </t>
-  </si>
-  <si>
-    <t>Estratégia de Ação</t>
-  </si>
-  <si>
-    <t>Mistura entre trabalho e estágio</t>
-  </si>
-  <si>
-    <t>Projeto inacabado, desmotivação, impossibilidade de finalizar o estágio.</t>
-  </si>
-  <si>
-    <t>Projeto</t>
-  </si>
-  <si>
-    <t>Realizar uma separação clara entre horas dedicadas para o trabalho normal diário e o tempo alocado para o desenvolvimento do estágio</t>
-  </si>
-  <si>
-    <t>Discordância com os stakeholders</t>
-  </si>
-  <si>
-    <t>Insucesso do projeto, alterações ao produto/projeto e atraso de prazos.</t>
-  </si>
-  <si>
-    <t>Projeto, Produto</t>
-  </si>
-  <si>
-    <t>Efetuar uma reunião com as partes interessadas</t>
-  </si>
-  <si>
-    <t>Problemas de hardware</t>
-  </si>
-  <si>
-    <t>Atraso no projeto, perda do desenvolvimento e progresso realizado e probabilidade de perda de equipamento.</t>
-  </si>
-  <si>
-    <t>Projeto, Produto e Recursos</t>
-  </si>
-  <si>
-    <t>Reparar ou adquirir novo hardware</t>
-  </si>
-  <si>
-    <t>Desmotivação</t>
-  </si>
-  <si>
-    <t>Atraso no projeto, atraso na entrega, possibilidade de não existir entrega.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fazer uma revisão ao projeto e realizar entregas mais frequentes aos stakeholders de forma a acrescentar mais valor ao produto e aumentar a interação com os stakeholders </t>
-  </si>
-  <si>
-    <t>Falta de skills</t>
-  </si>
-  <si>
-    <t>Atraso no projeto, projeto incompleto, com falhas.</t>
-  </si>
-  <si>
-    <t>Projeto e Produto</t>
-  </si>
-  <si>
-    <t>Solicitar ajuda ao supervisor, dedicar mais tempo para o desenvolvimento do projeto</t>
-  </si>
-  <si>
-    <t>Problemas de software</t>
-  </si>
-  <si>
-    <t>Atraso no projeto e complicações no desenvolvimento do produto.</t>
-  </si>
-  <si>
-    <t>Encontrar softwares alternativos, executar testes ao software</t>
-  </si>
-  <si>
-    <t>Covid19</t>
-  </si>
-  <si>
-    <t>Atraso no projeto, impossibilidade de desenvolvimento por tempo indeterminado.</t>
-  </si>
-  <si>
-    <t>Revisão do planeamento e tarefas. Escolha das tarefas prioritárias para o projeto</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>TEST CHECK</t>
   </si>
@@ -857,6 +747,18 @@
       </rPr>
       <t xml:space="preserve"> interativos compostos com gráficos e outras métricas de evolução, para que possa analisar tendências e pontos críticos de forma intuitiva.</t>
     </r>
+  </si>
+  <si>
+    <t>BURNDOWN CHART 2º SPRINT</t>
+  </si>
+  <si>
+    <t>BURNDOWN CHART 3º SPRINT</t>
+  </si>
+  <si>
+    <t>BURNDOWN CHART 4º SPRINT</t>
+  </si>
+  <si>
+    <t>BURNDOWN CHART 5º SPRINT</t>
   </si>
 </sst>
 </file>
@@ -1421,34 +1323,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1464,15 +1342,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1568,9 +1437,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1591,13 +1457,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Cabeçalho 1 2" xfId="1" xr:uid="{22A1AFC1-1147-4461-9DD1-CC7B48504495}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{EEC9C09B-E6E4-4B91-A270-87C046EE7CAA}"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1693,232 +1571,6 @@
           <bgColor rgb="FFFF5050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color auto="1"/>
-        </left>
-        <right style="medium">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8256,297 +7908,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="BURNDOWN CHART"/>
-      <sheetName val="PROJECT DETAILS"/>
-      <sheetName val="INSTRUCTIONS"/>
-      <sheetName val="RESOURCES"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="F8" t="str">
-            <v>Goal velocity</v>
-          </cell>
-          <cell r="G8" t="str">
-            <v>Remaining</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>1</v>
-          </cell>
-          <cell r="F9">
-            <v>32</v>
-          </cell>
-          <cell r="G9">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>2</v>
-          </cell>
-          <cell r="F10">
-            <v>30.45</v>
-          </cell>
-          <cell r="G10">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>3</v>
-          </cell>
-          <cell r="F11">
-            <v>28.9</v>
-          </cell>
-          <cell r="G11">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>4</v>
-          </cell>
-          <cell r="F12">
-            <v>27.349999999999998</v>
-          </cell>
-          <cell r="G12">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>5</v>
-          </cell>
-          <cell r="F13">
-            <v>25.799999999999997</v>
-          </cell>
-          <cell r="G13">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>6</v>
-          </cell>
-          <cell r="F14">
-            <v>24.249999999999996</v>
-          </cell>
-          <cell r="G14">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>7</v>
-          </cell>
-          <cell r="F15">
-            <v>22.699999999999996</v>
-          </cell>
-          <cell r="G15">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>8</v>
-          </cell>
-          <cell r="F16">
-            <v>21.149999999999995</v>
-          </cell>
-          <cell r="G16">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>9</v>
-          </cell>
-          <cell r="F17">
-            <v>19.599999999999994</v>
-          </cell>
-          <cell r="G17">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>10</v>
-          </cell>
-          <cell r="F18">
-            <v>18.049999999999994</v>
-          </cell>
-          <cell r="G18">
-            <v>32</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>11</v>
-          </cell>
-          <cell r="F19">
-            <v>16.499999999999993</v>
-          </cell>
-          <cell r="G19">
-            <v>29</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>12</v>
-          </cell>
-          <cell r="F20">
-            <v>14.999999999999993</v>
-          </cell>
-          <cell r="G20">
-            <v>29</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>13</v>
-          </cell>
-          <cell r="F21">
-            <v>13.499999999999993</v>
-          </cell>
-          <cell r="G21">
-            <v>25</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>14</v>
-          </cell>
-          <cell r="F22">
-            <v>11.999999999999993</v>
-          </cell>
-          <cell r="G22">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>15</v>
-          </cell>
-          <cell r="F23">
-            <v>10.499999999999993</v>
-          </cell>
-          <cell r="G23">
-            <v>20</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>16</v>
-          </cell>
-          <cell r="F24">
-            <v>8.9999999999999929</v>
-          </cell>
-          <cell r="G24">
-            <v>18</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>17</v>
-          </cell>
-          <cell r="F25">
-            <v>7.4999999999999929</v>
-          </cell>
-          <cell r="G25">
-            <v>14</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>18</v>
-          </cell>
-          <cell r="F26">
-            <v>5.9999999999999929</v>
-          </cell>
-          <cell r="G26">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>19</v>
-          </cell>
-          <cell r="F27">
-            <v>4.4999999999999929</v>
-          </cell>
-          <cell r="G27">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>20</v>
-          </cell>
-          <cell r="F28">
-            <v>2.9999999999999929</v>
-          </cell>
-          <cell r="G28">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>21</v>
-          </cell>
-          <cell r="F29">
-            <v>1.4999999999999929</v>
-          </cell>
-          <cell r="G29">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>22</v>
-          </cell>
-          <cell r="F30">
-            <v>0</v>
-          </cell>
-          <cell r="G30">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74E5AB98-80B4-47D5-8ABB-E0BA938354B9}" name="Table1" displayName="Table1" ref="B4:G11" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="B4:G11" xr:uid="{91071B6F-CF10-47B9-BE34-5BA8D31BDCA8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G11">
-    <sortCondition descending="1" ref="C4:C11"/>
-  </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8D52CB95-38F3-4FE7-9009-7AC6EF2EE5CF}" name="Risco" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{32FB5AF4-27C3-4F01-8E47-D25BEB490826}" name="Grau de Impacto" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{62E99B7D-20AF-4631-A714-B703B94F7F71}" name="Grau de Probabilidade" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{A7660C92-FB3C-422C-A058-506B15C34D1A}" name="Consequências" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{BD45F0D3-A83C-46A1-B7B6-E35C11F9A8BD}" name="Recursos Afetados " dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{9BFDFB35-E276-49AB-83AE-156D149A18D5}" name="Estratégia de Ação" dataDxfId="12"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -8863,620 +8224,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC2BA1F-6019-4F38-8DB8-E7A878F37D87}">
-  <dimension ref="B2:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79113791-FC73-4EB4-921D-87F49D6BBE25}">
-  <dimension ref="B3:J11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="28" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19" style="9" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:10" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="2:10" s="4" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6">
-        <v>5</v>
-      </c>
-      <c r="D5" s="6">
-        <v>4</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="2:10" s="4" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" s="4" customFormat="1" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="6">
-        <v>3</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="6">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="2:10" s="4" customFormat="1" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:G3"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B5:G11">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I9">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358BC198-B1EE-4A77-B085-0848BA011185}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="B1:T15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="75.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="123.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="128.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="123.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="128.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:20" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:20" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="2:20" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="2:20" s="12" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="7"/>
+      <c r="K7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="S8" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="7"/>
+      <c r="K9" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="5"/>
+      <c r="C10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="7"/>
+      <c r="K10" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="7"/>
+      <c r="K11" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="2:20" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="2:20" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="D13" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="7"/>
     </row>
-    <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+    <row r="14" spans="2:20" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="7"/>
     </row>
-    <row r="4" spans="2:20" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-    </row>
-    <row r="5" spans="2:20" s="23" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="22"/>
-    </row>
-    <row r="6" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13"/>
-      <c r="C6" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="15"/>
-      <c r="K6" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
-      <c r="C7" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="15"/>
-      <c r="K7" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q7" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="R7" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="T7" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="13"/>
-      <c r="C8" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="15"/>
-      <c r="K8" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="T8" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="13"/>
-      <c r="C9" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="15"/>
-      <c r="K9" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="R9" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="S9" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="T9" s="40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="13"/>
-      <c r="C10" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="15"/>
-      <c r="K10" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="N10" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q10" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="R10" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="S10" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="T10" s="40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="13"/>
-      <c r="C11" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="15"/>
-      <c r="K11" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="S11" s="2"/>
-    </row>
-    <row r="12" spans="2:20" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="13"/>
-      <c r="C12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="2:20" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="13"/>
-      <c r="C13" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="2:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="59"/>
+    <row r="15" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="46"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9539,33 +8637,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD6AECB-F8B7-4B06-AC7C-54A294647C38}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="B6:V15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="62" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" style="62"/>
-    <col min="5" max="5" width="16" style="62" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="62" customWidth="1"/>
-    <col min="8" max="16" width="8.6640625" style="62"/>
-    <col min="17" max="17" width="9.33203125" style="62" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="62"/>
+    <col min="1" max="1" width="4.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="50"/>
+    <col min="5" max="5" width="16" style="50" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="50" customWidth="1"/>
+    <col min="8" max="16" width="8.7109375" style="50"/>
+    <col min="17" max="17" width="9.28515625" style="50" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
@@ -9583,180 +8681,180 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>75</v>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="64">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
         <v>6</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="52">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="52">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="53">
         <v>12</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="53">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="64">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
         <v>7</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="52">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="53">
         <f>F9-D10</f>
         <v>10</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="53">
         <f>G9-E10</f>
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="64">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
         <v>8</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="52">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="53">
         <f t="shared" ref="F11:G15" si="0">F10-D11</f>
         <v>8</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="64">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
         <v>9</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="52">
         <v>2</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="52">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="64">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
         <v>10</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="52">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="64">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
         <v>11</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="52">
         <v>2</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="64">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
         <v>12</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="52">
         <v>7</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="52">
         <v>2</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="52">
         <v>0</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -9772,7 +8870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0FEE2E-429A-4384-AA2E-AD3649DF5000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -9780,25 +8878,25 @@
   <dimension ref="B6:V15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="62" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" style="62"/>
-    <col min="5" max="5" width="16" style="62" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="62" customWidth="1"/>
-    <col min="8" max="16" width="8.6640625" style="62"/>
-    <col min="17" max="17" width="9.33203125" style="62" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="62"/>
+    <col min="1" max="1" width="4.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="50"/>
+    <col min="5" max="5" width="16" style="50" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="50" customWidth="1"/>
+    <col min="8" max="16" width="8.7109375" style="50"/>
+    <col min="17" max="17" width="9.28515625" style="50" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
@@ -9816,180 +8914,180 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>75</v>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="64">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
         <v>13</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="52">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="52">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="53">
         <v>12</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="53">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="64">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
         <v>14</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="52">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="53">
         <f>F9-D10</f>
         <v>10</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="53">
         <f>G9-E10</f>
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="64">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
         <v>15</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="52">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="53">
         <f t="shared" ref="F11:G15" si="0">F10-D11</f>
         <v>8</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="64">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
         <v>16</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="52">
         <v>2</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="52">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="64">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
         <v>17</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="52">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="64">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
         <v>18</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="52">
         <v>2</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="64">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
         <v>19</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="52">
         <v>7</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="52">
         <v>2</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="52">
         <v>0</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -10005,7 +9103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371E675F-30BC-4357-8001-5C141349E35A}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -10013,25 +9111,25 @@
   <dimension ref="B6:V15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B15"/>
+      <selection activeCell="B6" sqref="B6:R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="62" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" style="62"/>
-    <col min="5" max="5" width="16" style="62" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="62" customWidth="1"/>
-    <col min="8" max="16" width="8.6640625" style="62"/>
-    <col min="17" max="17" width="9.33203125" style="62" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="62"/>
+    <col min="1" max="1" width="4.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="50"/>
+    <col min="5" max="5" width="16" style="50" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="50" customWidth="1"/>
+    <col min="8" max="16" width="8.7109375" style="50"/>
+    <col min="17" max="17" width="9.28515625" style="50" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
@@ -10049,180 +9147,180 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>75</v>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="64">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
         <v>20</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="52">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="52">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="53">
         <v>12</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="53">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="64">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
         <v>21</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="52">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="53">
         <f>F9-D10</f>
         <v>10</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="53">
         <f>G9-E10</f>
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="64">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
         <v>22</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="52">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="53">
         <f t="shared" ref="F11:G15" si="0">F10-D11</f>
         <v>8</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="64">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
         <v>23</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="52">
         <v>2</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="52">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="64">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
         <v>24</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="52">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="64">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
         <v>25</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="52">
         <v>2</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="64">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
         <v>26</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="52">
         <v>7</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="52">
         <v>2</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="52">
         <v>0</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -10238,7 +9336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2C9664-C336-4947-B9C9-D8C10C697E8C}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -10246,25 +9344,25 @@
   <dimension ref="B6:V15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+      <selection activeCell="B6" sqref="B6:R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="62" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" style="62"/>
-    <col min="5" max="5" width="16" style="62" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="62" customWidth="1"/>
-    <col min="8" max="16" width="8.6640625" style="62"/>
-    <col min="17" max="17" width="9.33203125" style="62" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="62"/>
+    <col min="1" max="1" width="4.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="50"/>
+    <col min="5" max="5" width="16" style="50" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="50" customWidth="1"/>
+    <col min="8" max="16" width="8.7109375" style="50"/>
+    <col min="17" max="17" width="9.28515625" style="50" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
@@ -10282,180 +9380,180 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>75</v>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="64">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
         <v>27</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="52">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="52">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="53">
         <v>12</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="53">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="64">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
         <v>28</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="52">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="53">
         <f>F9-D10</f>
         <v>10</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="53">
         <f>G9-E10</f>
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="64">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
         <v>29</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="52">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="53">
         <f t="shared" ref="F11:G15" si="0">F10-D11</f>
         <v>8</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="64">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
         <v>30</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="52">
         <v>2</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="52">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="53">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="64">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
         <v>1</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="52">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="64">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
         <v>2</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="52">
         <v>2</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="64">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
         <v>3</v>
       </c>
-      <c r="C15" s="64">
+      <c r="C15" s="52">
         <v>7</v>
       </c>
-      <c r="D15" s="64">
+      <c r="D15" s="52">
         <v>2</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="52">
         <v>0</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -10471,7 +9569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D4E848-FC93-40D1-A977-941B987FA5D5}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -10479,25 +9577,25 @@
   <dimension ref="B6:V14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="62" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="62" customWidth="1"/>
-    <col min="3" max="4" width="8.6640625" style="62"/>
-    <col min="5" max="5" width="16" style="62" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="62" customWidth="1"/>
-    <col min="8" max="16" width="8.6640625" style="62"/>
-    <col min="17" max="17" width="9.33203125" style="62" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="62"/>
+    <col min="1" max="1" width="4.140625" style="50" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="50" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="50"/>
+    <col min="5" max="5" width="16" style="50" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="50" customWidth="1"/>
+    <col min="8" max="16" width="8.7109375" style="50"/>
+    <col min="17" max="17" width="9.28515625" style="50" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="50"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:22" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="60" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
@@ -10515,158 +9613,158 @@
       <c r="P6" s="60"/>
       <c r="Q6" s="60"/>
       <c r="R6" s="60"/>
-      <c r="S6" s="61"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>75</v>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="64">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
         <v>4</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="52">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="52">
         <v>2</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="52">
         <v>0</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="53">
         <v>10</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="53">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="64">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
         <v>5</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="52">
         <v>2</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="52">
         <v>0</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="53">
         <f>F9-D10</f>
         <v>8</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="53">
         <f>G9-E10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="64">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
         <v>6</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="52">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="52">
         <v>0</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="53">
         <f t="shared" ref="F11:G14" si="0">F10-D11</f>
         <v>6</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="64">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
         <v>7</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="52">
         <v>2</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="52">
         <v>0</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="64">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
         <v>8</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="52">
         <v>2</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="52">
         <v>0</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="53">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="64">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
         <v>9</v>
       </c>
-      <c r="C14" s="64">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="52">
         <v>2</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="52">
         <v>0</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>

</xml_diff>